<commit_message>
attr, state, props ,event
</commit_message>
<xml_diff>
--- a/有好货页面/id_1908017/需求表格.xlsx
+++ b/有好货页面/id_1908017/需求表格.xlsx
@@ -115,7 +115,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +125,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -242,7 +248,7 @@
     <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -273,6 +279,7 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff70ad47"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>

</xml_diff>